<commit_message>
rebuild with struct and vector
</commit_message>
<xml_diff>
--- a/materials/新建 XLSX 工作表.xlsx
+++ b/materials/新建 XLSX 工作表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" activeTab="1"/>
+    <workbookView windowWidth="25600" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="180">
-  <si>
-    <t>text</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="207">
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>rebuild</t>
   </si>
   <si>
     <t>messageset</t>
@@ -123,6 +126,9 @@
     <t>[Q] 玩家档案</t>
   </si>
   <si>
+    <t>U    U      N    N       OOOO</t>
+  </si>
+  <si>
     <t>起始牌</t>
   </si>
   <si>
@@ -138,6 +144,9 @@
     <t>[A] 经典模式</t>
   </si>
   <si>
+    <t>U    U      NN   N      OO  OO</t>
+  </si>
+  <si>
     <t>玩家抽卡</t>
   </si>
   <si>
@@ -150,6 +159,9 @@
     <t>[S] 趣味模式</t>
   </si>
   <si>
+    <t>U    U      N N  N      O    O</t>
+  </si>
+  <si>
     <t>不能UNO</t>
   </si>
   <si>
@@ -165,15 +177,24 @@
     <t>[D] 联机模式</t>
   </si>
   <si>
+    <t>U    U      N  N N      O    O</t>
+  </si>
+  <si>
     <t>UNO检举</t>
   </si>
   <si>
     <t>[F] 游戏设置</t>
   </si>
   <si>
+    <t>UU  UU      N   NN      OO  OO</t>
+  </si>
+  <si>
     <t>不能出牌</t>
   </si>
   <si>
+    <t xml:space="preserve"> UUUU       N    N       OOOO</t>
+  </si>
+  <si>
     <t>换色</t>
   </si>
   <si>
@@ -195,6 +216,9 @@
     <t>电 脑 数 量</t>
   </si>
   <si>
+    <t>[D] 无尽模式</t>
+  </si>
+  <si>
     <t>电 脑 难 度</t>
   </si>
   <si>
@@ -210,6 +234,9 @@
     <t>[D] 高级设置</t>
   </si>
   <si>
+    <t>[^] [v] [&lt;] [&gt;]</t>
+  </si>
+  <si>
     <t>随 机</t>
   </si>
   <si>
@@ -234,6 +261,9 @@
     <t>电 脑</t>
   </si>
   <si>
+    <t>〇</t>
+  </si>
+  <si>
     <t>[A] 普通设置</t>
   </si>
   <si>
@@ -600,34 +630,85 @@
     <t>|余XX牌|</t>
   </si>
   <si>
+    <t>\--/</t>
+  </si>
+  <si>
+    <t>U    U</t>
+  </si>
+  <si>
+    <t>N    N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OOOO</t>
+  </si>
+  <si>
+    <t>普通菜单</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
-    <t>\--/</t>
+    <t>NN   N</t>
+  </si>
+  <si>
+    <t>OO  OO</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>N N  N</t>
+  </si>
+  <si>
+    <t>O    O</t>
   </si>
   <si>
     <t>|</t>
   </si>
   <si>
+    <t>N  N N</t>
+  </si>
+  <si>
     <t>|基础信息|</t>
   </si>
   <si>
+    <t>UU  UU</t>
+  </si>
+  <si>
+    <t>N   NN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UUUU</t>
+  </si>
+  <si>
     <t>|牌局信息|</t>
   </si>
   <si>
+    <t>人类</t>
+  </si>
+  <si>
+    <t>电脑</t>
+  </si>
+  <si>
+    <t>难度</t>
+  </si>
+  <si>
     <t>[A]</t>
   </si>
   <si>
+    <t>牌组</t>
+  </si>
+  <si>
     <t>[S]</t>
   </si>
   <si>
+    <t>[D]</t>
+  </si>
+  <si>
     <t>第XX页/共XX页</t>
   </si>
   <si>
     <t>上一页[]</t>
-  </si>
-  <si>
-    <t>[D]</t>
   </si>
   <si>
     <t>第一页[]</t>
@@ -1724,14 +1805,15 @@
   <sheetPr/>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.6272727272727" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="15.625" customWidth="1"/>
-    <col min="7" max="16384" width="15.625" customWidth="1"/>
+    <col min="1" max="2" width="15.6272727272727" customWidth="1"/>
+    <col min="3" max="3" width="48.5454545454545" customWidth="1"/>
+    <col min="7" max="16384" width="15.6272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:10">
@@ -1739,18 +1821,21 @@
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:10">
@@ -1758,26 +1843,29 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H2" s="10" t="str">
         <f>_xlfn.DISPIMG("ID_DC9EB24FA76245B9A3BC3739A6A3F167",1)</f>
         <v>=DISPIMG("ID_DC9EB24FA76245B9A3BC3739A6A3F167",1)</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:10">
@@ -1785,26 +1873,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H3" s="10" t="str">
         <f>_xlfn.DISPIMG("ID_C8E69B7D29C14073A10E40D927E56094",1)</f>
         <v>=DISPIMG("ID_C8E69B7D29C14073A10E40D927E56094",1)</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:10">
@@ -1812,26 +1903,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H4" s="10" t="str">
         <f>_xlfn.DISPIMG("ID_5956D82EF0CB445AA418E0295D169E80",1)</f>
         <v>=DISPIMG("ID_5956D82EF0CB445AA418E0295D169E80",1)</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -1839,13 +1933,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -1853,13 +1950,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
       </c>
       <c r="D6">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -1867,13 +1967,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -1881,13 +1984,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
       </c>
       <c r="D8">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
@@ -1895,229 +2001,313 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:3">
       <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:2">
+        <v>35</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:3">
       <c r="A11" s="10">
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="1:2">
+        <v>36</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:3">
       <c r="A12" s="10">
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:2">
+        <v>38</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:3">
       <c r="A13" s="10">
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:2">
+        <v>39</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:3">
       <c r="A14" s="10">
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" customHeight="1" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:3">
       <c r="A15" s="10">
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:2">
+    <row r="16" customHeight="1" spans="1:3">
       <c r="A16" s="10">
         <v>14</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" customHeight="1" spans="1:2">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:3">
       <c r="A17" s="10">
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" customHeight="1" spans="1:2">
+    <row r="18" customHeight="1" spans="1:3">
       <c r="A18" s="10">
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" customHeight="1" spans="1:2">
+    <row r="19" customHeight="1" spans="1:3">
       <c r="A19" s="10">
         <v>17</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="1:2">
+        <v>46</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:3">
       <c r="A20" s="10">
         <v>18</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="1:2">
+        <v>47</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:3">
       <c r="A21" s="10">
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:2">
+        <v>48</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:3">
       <c r="A22" s="10">
         <v>20</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" customHeight="1" spans="1:2">
+        <v>49</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:3">
       <c r="A23" s="10">
         <v>21</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" customHeight="1" spans="1:2">
+        <v>50</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:3">
       <c r="A24" s="10">
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" customHeight="1" spans="1:2">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:3">
       <c r="A25" s="10">
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" customHeight="1" spans="1:2">
+        <v>53</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:3">
       <c r="A26" s="10">
         <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" customHeight="1" spans="1:2">
+        <v>54</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:3">
       <c r="A27" s="10">
         <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" customHeight="1" spans="1:2">
+        <v>11</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:3">
       <c r="A28" s="10">
         <v>26</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" customHeight="1" spans="1:2">
+        <v>55</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:3">
       <c r="A29" s="10">
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" customHeight="1" spans="1:2">
+        <v>56</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:3">
       <c r="A30" s="10">
         <v>28</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" customHeight="1" spans="1:2">
+        <v>57</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="1:3">
       <c r="A31" s="10">
         <v>29</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" customHeight="1" spans="1:2">
+        <v>58</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:3">
       <c r="A32" s="10">
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" customHeight="1" spans="1:2">
+        <v>59</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:3">
       <c r="A33" s="10">
         <v>31</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" customHeight="1" spans="1:2">
+        <v>60</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" customHeight="1" spans="1:3">
       <c r="A34" s="10">
         <v>32</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" customHeight="1" spans="1:2">
+        <v>61</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:3">
       <c r="A35" s="10">
         <v>33</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="36" customHeight="1" spans="1:2">
+        <v>62</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:3">
       <c r="A36" s="10">
         <v>34</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>53</v>
+        <v>63</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" customHeight="1" spans="1:2">
@@ -2125,7 +2315,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="1:2">
@@ -2133,7 +2323,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="1:2">
@@ -2141,7 +2331,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" customHeight="1" spans="1:2">
@@ -2149,7 +2339,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="1:2">
@@ -2157,7 +2347,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="1:2">
@@ -2165,7 +2355,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" customHeight="1" spans="1:2">
@@ -2173,7 +2363,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" customHeight="1" spans="1:2">
@@ -2181,7 +2371,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" customHeight="1" spans="1:2">
@@ -2189,7 +2379,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" customHeight="1" spans="1:2">
@@ -2197,7 +2387,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="1:2">
@@ -2205,7 +2395,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="1:2">
@@ -2213,7 +2403,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" customHeight="1" spans="1:2">
@@ -2221,7 +2411,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" customHeight="1" spans="1:2">
@@ -2229,7 +2419,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" customHeight="1" spans="1:2">
@@ -2237,7 +2427,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" customHeight="1" spans="1:2">
@@ -2245,7 +2435,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" customHeight="1" spans="1:2">
@@ -2253,7 +2443,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" customHeight="1" spans="1:2">
@@ -2261,7 +2451,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" customHeight="1" spans="1:2">
@@ -2269,7 +2459,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" customHeight="1" spans="1:2">
@@ -2277,7 +2467,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" customHeight="1" spans="1:2">
@@ -2285,7 +2475,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" customHeight="1" spans="1:2">
@@ -2293,7 +2483,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" customHeight="1" spans="1:2">
@@ -2301,7 +2491,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" customHeight="1" spans="1:2">
@@ -2309,7 +2499,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="61" customHeight="1" spans="1:2">
@@ -2317,7 +2507,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" customHeight="1" spans="1:2">
@@ -2325,7 +2515,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" customHeight="1" spans="1:2">
@@ -2333,7 +2523,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" customHeight="1" spans="1:2">
@@ -2341,7 +2531,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" customHeight="1" spans="1:2">
@@ -2349,7 +2539,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" customHeight="1" spans="1:2">
@@ -2357,7 +2547,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" customHeight="1" spans="1:2">
@@ -2365,7 +2555,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" customHeight="1" spans="1:2">
@@ -2373,7 +2563,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" customHeight="1" spans="1:2">
@@ -2381,7 +2571,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" customHeight="1" spans="1:2">
@@ -2389,7 +2579,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" customHeight="1" spans="1:2">
@@ -2397,7 +2587,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" customHeight="1" spans="1:2">
@@ -2405,7 +2595,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" customHeight="1" spans="1:2">
@@ -2413,7 +2603,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" customHeight="1" spans="1:2">
@@ -2421,7 +2611,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" customHeight="1" spans="1:2">
@@ -2429,7 +2619,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" customHeight="1" spans="1:2">
@@ -2437,7 +2627,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" customHeight="1" spans="1:2">
@@ -2445,7 +2635,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" customHeight="1" spans="1:2">
@@ -2453,7 +2643,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" customHeight="1" spans="1:2">
@@ -2461,7 +2651,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" customHeight="1" spans="1:2">
@@ -2469,7 +2659,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" customHeight="1" spans="1:2">
@@ -2477,7 +2667,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" customHeight="1" spans="1:2">
@@ -2485,7 +2675,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" customHeight="1" spans="1:2">
@@ -2493,7 +2683,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" customHeight="1" spans="1:2">
@@ -2501,7 +2691,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2516,11 +2706,11 @@
   <sheetPr/>
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" customFormat="1" spans="1:19">
       <c r="A1" s="1">
@@ -2583,61 +2773,61 @@
     </row>
     <row r="2" customFormat="1" spans="1:19">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="L2" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="M2" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="N2" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="O2" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="P2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="Q2" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="R2" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="S2" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:19">
@@ -2701,61 +2891,61 @@
     </row>
     <row r="5" customFormat="1" spans="1:19">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="J5" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="L5" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="M5" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="N5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="O5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="P5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="Q5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="R5" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="S5" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:19">
@@ -2819,61 +3009,61 @@
     </row>
     <row r="8" customFormat="1" spans="1:19">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="H8" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J8" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="K8" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="L8" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="M8" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="N8" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="O8" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="P8" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="Q8" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="R8" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="S8" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:19">
@@ -2937,64 +3127,64 @@
     </row>
     <row r="11" customFormat="1" spans="1:19">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="H11" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="I11" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="J11" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="K11" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="L11" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="M11" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="N11" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="O11" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="P11" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="Q11" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="R11" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="S11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" ht="14.75"/>
     <row r="13" customFormat="1" spans="1:9">
       <c r="A13">
         <v>110</v>
@@ -3018,30 +3208,30 @@
         <v>198</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:9">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I14" s="8"/>
     </row>
@@ -3075,25 +3265,25 @@
     </row>
     <row r="17" customFormat="1" spans="1:9">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I17" s="8"/>
     </row>
@@ -3127,25 +3317,25 @@
     </row>
     <row r="20" customFormat="1" spans="1:9">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E20" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="F20" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I20" s="8"/>
     </row>
@@ -3177,27 +3367,27 @@
       </c>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" customFormat="1" ht="14.25" spans="1:9">
+    <row r="23" customFormat="1" ht="14.75" spans="1:9">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="F23" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I23" s="9"/>
     </row>
@@ -3229,28 +3419,28 @@
     </row>
     <row r="26" customFormat="1" spans="1:8">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B26" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C26" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E26" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G26" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="H26" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3266,26 +3456,32 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" s="14" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="F1">
         <v>118</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="6:8">
@@ -3293,167 +3489,230 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="F3">
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="F4">
         <f>F1-F2*F3</f>
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F5">
         <f>F4/(F2+1)</f>
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="I5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="H6" t="s">
-        <v>158</v>
-      </c>
-      <c r="M6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="M7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="8:13">
+        <v>167</v>
+      </c>
+      <c r="N7" t="s">
+        <v>176</v>
+      </c>
+      <c r="O7" t="s">
+        <v>177</v>
+      </c>
+      <c r="P7" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="8:17">
       <c r="H8" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="K8" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="L8" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="M8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13">
+        <v>180</v>
+      </c>
+      <c r="N8" t="s">
+        <v>176</v>
+      </c>
+      <c r="O8" t="s">
+        <v>181</v>
+      </c>
+      <c r="P8" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16">
       <c r="C9" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="M9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>180</v>
+      </c>
+      <c r="N9" t="s">
+        <v>176</v>
+      </c>
+      <c r="O9" t="s">
+        <v>184</v>
+      </c>
+      <c r="P9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>180</v>
+      </c>
+      <c r="N10" t="s">
+        <v>176</v>
+      </c>
+      <c r="O10" t="s">
+        <v>187</v>
+      </c>
+      <c r="P10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="M11" t="s">
+        <v>180</v>
+      </c>
+      <c r="N11" t="s">
+        <v>189</v>
+      </c>
+      <c r="O11" t="s">
+        <v>190</v>
+      </c>
+      <c r="P11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="M12" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" t="s">
+        <v>191</v>
+      </c>
+      <c r="O12" t="s">
+        <v>177</v>
+      </c>
+      <c r="P12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
+      <c r="Q13" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:13">
+    <row r="15" spans="3:17">
       <c r="C15" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H15">
         <v>6</v>
       </c>
-      <c r="M15" t="s">
-        <v>170</v>
+      <c r="Q15" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="8:8">
@@ -3461,111 +3720,141 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="H17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="Q17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="H18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="N18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="M19" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="H20">
         <v>11</v>
       </c>
-      <c r="M20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="N20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H21">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="8:8">
+      <c r="M21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="8:14">
       <c r="H22">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="N22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="14" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="H23">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="M23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
+        <v>167</v>
+      </c>
+      <c r="N24" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>173</v>
-      </c>
-      <c r="M25" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
       <c r="H26" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="I26" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="H28" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="14" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="M30" s="14" t="s">
-        <v>157</v>
+        <v>167</v>
+      </c>
+      <c r="N30" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q30" s="14" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>